<commit_message>
updated goat, moose transect, and elk general
</commit_message>
<xml_diff>
--- a/utils/templates/observations/transform/input/Goat_test.xlsx
+++ b/utils/templates/observations/transform/input/Goat_test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anissa/Desktop/BHBC-1412:BHBC-1974/Goat/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anissa/DevelopmentProjects/biohubbc-utils/utils/templates/observations/transform/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC41139E-075E-B040-99A3-EAE796B415E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7A7F2B-E534-FF45-9DED-AD542603C2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18940" yWindow="-20540" windowWidth="23260" windowHeight="12580" tabRatio="672" activeTab="2" xr2:uid="{EA928297-87AF-4A2F-92BD-649BD8B345BB}"/>
+    <workbookView xWindow="-18940" yWindow="-20540" windowWidth="29020" windowHeight="16800" tabRatio="672" activeTab="1" xr2:uid="{EA928297-87AF-4A2F-92BD-649BD8B345BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Effort &amp; Site Conditions" sheetId="2" r:id="rId1"/>
@@ -1895,7 +1895,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="376">
   <si>
     <t>Date</t>
   </si>
@@ -3023,33 +3023,6 @@
   </si>
   <si>
     <t>marked_comment_1</t>
-  </si>
-  <si>
-    <t>WHID2</t>
-  </si>
-  <si>
-    <t>BH002</t>
-  </si>
-  <si>
-    <t>7C28091</t>
-  </si>
-  <si>
-    <t>150.155</t>
-  </si>
-  <si>
-    <t>right_ear_tag_2</t>
-  </si>
-  <si>
-    <t>right_ear_color_2</t>
-  </si>
-  <si>
-    <t>left_ear_tag_2</t>
-  </si>
-  <si>
-    <t>left_ear_color_2</t>
-  </si>
-  <si>
-    <t>marked_comment_2</t>
   </si>
 </sst>
 </file>
@@ -17940,8 +17913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CACE0D7-C202-416C-A799-EE712DC4F630}">
   <dimension ref="A1:AG501"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -25729,10 +25702,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7C5C50-7D41-4386-95DF-AC97EF3E04C6}">
-  <dimension ref="A1:M104"/>
+  <dimension ref="A1:M103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -25832,46 +25805,18 @@
         <v>375</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
-        <v>364</v>
-      </c>
-      <c r="B3" s="56">
-        <v>43523</v>
-      </c>
-      <c r="C3" s="37" t="s">
-        <v>213</v>
-      </c>
-      <c r="D3" s="29" t="s">
-        <v>376</v>
-      </c>
-      <c r="E3" s="37" t="s">
-        <v>377</v>
-      </c>
-      <c r="F3" s="29" t="s">
-        <v>378</v>
-      </c>
-      <c r="G3" s="38" t="s">
-        <v>379</v>
-      </c>
-      <c r="H3" s="30" t="s">
-        <v>244</v>
-      </c>
-      <c r="I3" s="29" t="s">
-        <v>380</v>
-      </c>
-      <c r="J3" s="29" t="s">
-        <v>381</v>
-      </c>
-      <c r="K3" s="29" t="s">
-        <v>382</v>
-      </c>
-      <c r="L3" s="29" t="s">
-        <v>383</v>
-      </c>
-      <c r="M3" s="29" t="s">
-        <v>384</v>
-      </c>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="29"/>
+      <c r="B3" s="31"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="29"/>
@@ -27173,19 +27118,6 @@
       <c r="L103" s="29"/>
       <c r="M103" s="29"/>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A104" s="29"/>
-      <c r="B104" s="31"/>
-      <c r="D104" s="29"/>
-      <c r="E104" s="29"/>
-      <c r="F104" s="29"/>
-      <c r="G104" s="29"/>
-      <c r="I104" s="29"/>
-      <c r="J104" s="29"/>
-      <c r="K104" s="29"/>
-      <c r="L104" s="29"/>
-      <c r="M104" s="29"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -27197,13 +27129,13 @@
           <x14:formula1>
             <xm:f>'Picklist Values'!$N$2:$N$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C4:C104</xm:sqref>
+          <xm:sqref>C3:C103</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4DC65864-BD41-4D75-BE64-3FA004431512}">
           <x14:formula1>
             <xm:f>'Picklist Values'!$P$2:$P$4</xm:f>
           </x14:formula1>
-          <xm:sqref>H4:H104</xm:sqref>
+          <xm:sqref>H3:H103</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>